<commit_message>
Reporting Result of Researching by Letu_V5 Algorithm
</commit_message>
<xml_diff>
--- a/Отчет_4_сем/Сравнительные результаты LETU_v5.xlsx
+++ b/Отчет_4_сем/Сравнительные результаты LETU_v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FavouritesFolders\Documents\GitHub\MastersDegree\Отчет_4_сем\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBF4AD3-0D81-4291-8BAD-94BD0BAFE48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719FE1F2-2611-48E6-A3CB-A1D7A06174EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,25 +25,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">	Qini curve AUC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">	UpLift curve AUC </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Структура</t>
   </si>
   <si>
     <t>Базовое решение</t>
+  </si>
+  <si>
+    <t>Решение с одной моделью</t>
+  </si>
+  <si>
+    <t>Решение с двумя независимыми моделями</t>
+  </si>
+  <si>
+    <t>Трансформация класса в задачу классификации</t>
+  </si>
+  <si>
+    <t>Трансформация класса в задачу регрессии</t>
+  </si>
+  <si>
+    <t>Решение с одной моделью с поиском лучшей модели</t>
+  </si>
+  <si>
+    <t>Трансформация класса в задачу регрессии с поиском лучшей модели</t>
+  </si>
+  <si>
+    <t>UpLift curve AUC</t>
+  </si>
+  <si>
+    <t>Qini curve AUC</t>
+  </si>
+  <si>
+    <t>Номер</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +82,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -67,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -75,13 +106,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -103,16 +331,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>259556</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>333374</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -152,8 +380,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="723900" y="95250"/>
-          <a:ext cx="809625" cy="228600"/>
+          <a:off x="10270331" y="333374"/>
+          <a:ext cx="902494" cy="238126"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,39 +666,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1.6149999999999999E-3</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4.0900000000000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.23E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="15">
         <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.44E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.24E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.38E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.55E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="16">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>7.7000000000000002E-3</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D3:F9 C10:C1048576 D2:D9">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{397660DF-9617-41C7-AC63-66FFF543EA51}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E9 D10:D1048576">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{92B3CAFD-35EF-41B4-9B81-502C6E608F4A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9 E10:E12 E21:E1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{41B46D8F-1DB0-470F-9BA9-62866E778691}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{397660DF-9617-41C7-AC63-66FFF543EA51}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D3:F9 C10:C1048576 D2:D9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{92B3CAFD-35EF-41B4-9B81-502C6E608F4A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E2:E9 D10:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{41B46D8F-1DB0-470F-9BA9-62866E778691}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F2:F9 E10:E12 E21:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>